<commit_message>
Completed merge with remote
</commit_message>
<xml_diff>
--- a/project1/runs/tsqr/TSQR_Analysis.xlsx
+++ b/project1/runs/tsqr/TSQR_Analysis.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Desktop\Coding\MATH-505\project1\runs\tsqr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05534059-3192-43A9-AC0E-DC78D906CD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F7FE58-679C-44E2-AAC2-930E3D63740A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{7B4D1BD7-DBA4-43C2-A926-556BA9DBD68C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{7B4D1BD7-DBA4-43C2-A926-556BA9DBD68C}"/>
   </bookViews>
   <sheets>
     <sheet name="tsqr_results" sheetId="2" r:id="rId1"/>
     <sheet name="tsqr_sparse_results" sheetId="3" r:id="rId2"/>
     <sheet name="Sequential Runs" sheetId="1" r:id="rId3"/>
+    <sheet name="Parallel Runs" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">tsqr_results!$A$1:$D$45</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Column1</t>
   </si>
@@ -798,7 +799,7 @@
                   <c:v>14.784371681750001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.346810432250003</c:v>
+                  <c:v>17.166546010666668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -814,7 +815,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sequential Runs'!$A$15</c:f>
+              <c:f>'Sequential Runs'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -908,7 +909,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Sequential Runs'!$F$16,'Sequential Runs'!$F$20,'Sequential Runs'!$F$24)</c:f>
+              <c:f>('Sequential Runs'!$F$15,'Sequential Runs'!$F$19,'Sequential Runs'!$F$23)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -935,7 +936,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sequential Runs'!$A$29</c:f>
+              <c:f>'Sequential Runs'!$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -960,7 +961,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="3.6111111111111108E-2"/>
-                  <c:y val="-"/>
+                  <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="outEnd"/>
@@ -1051,7 +1052,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Sequential Runs'!$F$30,'Sequential Runs'!$F$34,'Sequential Runs'!$F$38)</c:f>
+              <c:f>('Sequential Runs'!$F$29,'Sequential Runs'!$F$33,'Sequential Runs'!$F$37)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1577,7 +1578,7 @@
                   <c:v>14.784371681750001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.346810432250003</c:v>
+                  <c:v>17.166546010666668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1593,7 +1594,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sequential Runs'!$A$15</c:f>
+              <c:f>'Sequential Runs'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1753,7 +1754,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Sequential Runs'!$F$16,'Sequential Runs'!$F$20,'Sequential Runs'!$F$24)</c:f>
+              <c:f>('Sequential Runs'!$F$15,'Sequential Runs'!$F$19,'Sequential Runs'!$F$23)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1780,7 +1781,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sequential Runs'!$A$29</c:f>
+              <c:f>'Sequential Runs'!$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1940,7 +1941,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Sequential Runs'!$F$30,'Sequential Runs'!$F$34,'Sequential Runs'!$F$38)</c:f>
+              <c:f>('Sequential Runs'!$F$29,'Sequential Runs'!$F$33,'Sequential Runs'!$F$37)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2124,7 +2125,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Execution Time (seconds Log10 scale)</a:t>
+                  <a:t>Execution Time (seconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2158,7 +2159,870 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="314582943"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Parallel Runtime</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sequential Runs'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TSQR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>30</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>40</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Parallel Runs'!$F$36,'Parallel Runs'!$F$41,'Parallel Runs'!$F$46)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.5542988141999983</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.933981522399999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8269493228</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2F28-4B93-B732-235D5128184A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Parallel Runs'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CQR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.209361342352285E-2"/>
+                  <c:y val="-9.4427793594226664E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-2F28-4B93-B732-235D5128184A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.4855315101463181E-2"/>
+                  <c:y val="-8.4985014234804007E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-2F28-4B93-B732-235D5128184A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.485531510146308E-2"/>
+                  <c:y val="-8.0263624555092672E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-2F28-4B93-B732-235D5128184A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>30</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>40</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Parallel Runs'!$F$2,'Parallel Runs'!$F$7,'Parallel Runs'!$F$12)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.8098226400000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9355168600000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7960221399999993E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2F28-4B93-B732-235D5128184A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sequential Runs'!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CGS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-2F28-4B93-B732-235D5128184A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.5000000000000001E-2"/>
+                  <c:y val="-8.7962962962962965E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-2F28-4B93-B732-235D5128184A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>30</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>40</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>50</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Parallel Runs'!$F$19,'Parallel Runs'!$F$24,'Parallel Runs'!$F$29)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.7657274200000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4333150599999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12607392079999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-2F28-4B93-B732-235D5128184A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="314582943"/>
+        <c:axId val="314583903"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="314582943"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Matrix Choice</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="314583903"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="314583903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Execution Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2399,6 +3263,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3419,6 +4323,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3969,12 +5376,12 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4004,13 +5411,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4033,6 +5440,49 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>326796</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>149886</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{984703F9-367E-4362-B376-538D00A4C410}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5528,10 +6978,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6849AA5-9B5A-4B32-A374-7F4DA4F2AF0C}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="97" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView topLeftCell="A3" zoomScale="78" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5564,7 +7014,7 @@
         <v>9.4428551515657096E-13</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="G2:I2" si="0">AVERAGE(C2:C5)</f>
+        <f t="shared" ref="H2:I2" si="0">AVERAGE(C2:C5)</f>
         <v>41.471548229814204</v>
       </c>
       <c r="I2" s="1">
@@ -5732,20 +7182,20 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
-        <f>AVERAGE(A10:A13)</f>
-        <v>17.346810432250003</v>
+        <f>AVERAGE(A10:A12)</f>
+        <v>17.166546010666668</v>
       </c>
       <c r="G10" s="1">
-        <f>AVERAGE(B10:B13)</f>
+        <f>AVERAGE(B10:B12)</f>
         <v>9.384750035259759E-13</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10" si="4">AVERAGE(C10:C13)</f>
+        <f>AVERAGE(C10:C12)</f>
         <v>1328.3759059912099</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" ref="I10" si="5">AVERAGE(D10:D13)</f>
-        <v>0.21123315007771437</v>
+        <f>AVERAGE(D10:D12)</f>
+        <v>8.4493260031060402E-14</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -5769,7 +7219,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>17.887603696999999</v>
+        <v>16.573857306000001</v>
       </c>
       <c r="B12" s="1">
         <v>9.384750035259759E-13</v>
@@ -5778,7 +7228,7 @@
         <v>1328.3759059912099</v>
       </c>
       <c r="D12" s="1">
-        <v>0.84493260031060402</v>
+        <v>8.4493260031060402E-14</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5787,42 +7237,54 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>16.573857306000001</v>
-      </c>
-      <c r="B13" s="1">
-        <v>9.384750035259759E-13</v>
-      </c>
-      <c r="C13">
-        <v>1328.3759059912099</v>
-      </c>
-      <c r="D13" s="1">
-        <v>8.4493260031060402E-14</v>
-      </c>
-      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="A15">
+        <v>2.1450218E-2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0015167662756799E-12</v>
+      </c>
+      <c r="C15">
+        <v>41.4710403851536</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.5642377328759599E-13</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <f>AVERAGE(A15:A18)</f>
+        <v>1.7381321999999998E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" ref="G15" si="4">AVERAGE(B15:B18)</f>
+        <v>1.0015167662756799E-12</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" ref="H15" si="5">AVERAGE(C15:C18)</f>
+        <v>41.4710403851536</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" ref="I15" si="6">AVERAGE(D15:D18)</f>
+        <v>1.5642377328759599E-13</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2.1450218E-2</v>
+        <v>1.5123968999999999E-2</v>
       </c>
       <c r="B16" s="1">
         <v>1.0015167662756799E-12</v>
@@ -5834,26 +7296,14 @@
         <v>1.5642377328759599E-13</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <f>AVERAGE(A16:A19)</f>
-        <v>1.7381321999999998E-2</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" ref="G16" si="6">AVERAGE(B16:B19)</f>
-        <v>1.0015167662756799E-12</v>
-      </c>
-      <c r="H16" s="1">
-        <f t="shared" ref="H16" si="7">AVERAGE(C16:C19)</f>
-        <v>41.4710403851536</v>
-      </c>
-      <c r="I16" s="1">
-        <f t="shared" ref="I16" si="8">AVERAGE(D16:D19)</f>
-        <v>1.5642377328759599E-13</v>
-      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>1.5123968999999999E-2</v>
+        <v>1.6580437E-2</v>
       </c>
       <c r="B17" s="1">
         <v>1.0015167662756799E-12</v>
@@ -5872,7 +7322,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>1.6580437E-2</v>
+        <v>1.6370664E-2</v>
       </c>
       <c r="B18" s="1">
         <v>1.0015167662756799E-12</v>
@@ -5891,26 +7341,38 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>1.6370664E-2</v>
+        <v>2.1543336E-2</v>
       </c>
       <c r="B19" s="1">
-        <v>1.0015167662756799E-12</v>
+        <v>1.61398067363638E-12</v>
       </c>
       <c r="C19">
-        <v>41.4710403851536</v>
+        <v>411.653612574921</v>
       </c>
       <c r="D19" s="1">
-        <v>1.5642377328759599E-13</v>
+        <v>1.5725097269031499E-11</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="F19" s="1">
+        <f>AVERAGE(A19:A22)</f>
+        <v>2.2947338249999998E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" ref="G19" si="7">AVERAGE(B19:B22)</f>
+        <v>1.61398067363638E-12</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" ref="H19" si="8">AVERAGE(C19:C22)</f>
+        <v>411.653612574921</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" ref="I19" si="9">AVERAGE(D19:D22)</f>
+        <v>1.5725097269031499E-11</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>2.1543336E-2</v>
+        <v>2.3557066000000002E-2</v>
       </c>
       <c r="B20" s="1">
         <v>1.61398067363638E-12</v>
@@ -5922,26 +7384,14 @@
         <v>1.5725097269031499E-11</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="1">
-        <f>AVERAGE(A20:A23)</f>
-        <v>2.2947338249999998E-2</v>
-      </c>
-      <c r="G20" s="1">
-        <f t="shared" ref="G20" si="9">AVERAGE(B20:B23)</f>
-        <v>1.61398067363638E-12</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" ref="H20" si="10">AVERAGE(C20:C23)</f>
-        <v>411.653612574921</v>
-      </c>
-      <c r="I20" s="1">
-        <f t="shared" ref="I20" si="11">AVERAGE(D20:D23)</f>
-        <v>1.5725097269031499E-11</v>
-      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>2.3557066000000002E-2</v>
+        <v>2.1273824E-2</v>
       </c>
       <c r="B21" s="1">
         <v>1.61398067363638E-12</v>
@@ -5960,7 +7410,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>2.1273824E-2</v>
+        <v>2.5415126999999999E-2</v>
       </c>
       <c r="B22" s="1">
         <v>1.61398067363638E-12</v>
@@ -5979,26 +7429,38 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>2.5415126999999999E-2</v>
+        <v>2.8815963999999999E-2</v>
       </c>
       <c r="B23" s="1">
-        <v>1.61398067363638E-12</v>
+        <v>6.7303634028587697E-12</v>
       </c>
       <c r="C23">
-        <v>411.653612574921</v>
+        <v>1328.4253613137801</v>
       </c>
       <c r="D23" s="1">
-        <v>1.5725097269031499E-11</v>
+        <v>4.8176401812824898E-11</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="F23" s="1">
+        <f>AVERAGE(A23:A26)</f>
+        <v>2.9412260250000002E-2</v>
+      </c>
+      <c r="G23" s="1">
+        <f>AVERAGE(B23:B26)</f>
+        <v>6.7303634028587697E-12</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" ref="H23" si="10">AVERAGE(C23:C26)</f>
+        <v>1328.4253613137801</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" ref="I23" si="11">AVERAGE(D23:D26)</f>
+        <v>4.8176401812824898E-11</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>2.8815963999999999E-2</v>
+        <v>3.0480533000000001E-2</v>
       </c>
       <c r="B24" s="1">
         <v>6.7303634028587697E-12</v>
@@ -6010,26 +7472,14 @@
         <v>4.8176401812824898E-11</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="1">
-        <f>AVERAGE(A24:A27)</f>
-        <v>2.9412260250000002E-2</v>
-      </c>
-      <c r="G24" s="1">
-        <f>AVERAGE(B24:B27)</f>
-        <v>6.7303634028587697E-12</v>
-      </c>
-      <c r="H24" s="1">
-        <f t="shared" ref="H24" si="12">AVERAGE(C24:C27)</f>
-        <v>1328.4253613137801</v>
-      </c>
-      <c r="I24" s="1">
-        <f t="shared" ref="I24" si="13">AVERAGE(D24:D27)</f>
-        <v>4.8176401812824898E-11</v>
-      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>3.0480533000000001E-2</v>
+        <v>2.9237602000000001E-2</v>
       </c>
       <c r="B25" s="1">
         <v>6.7303634028587697E-12</v>
@@ -6048,7 +7498,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>2.9237602000000001E-2</v>
+        <v>2.9114942000000001E-2</v>
       </c>
       <c r="B26" s="1">
         <v>6.7303634028587697E-12</v>
@@ -6066,42 +7516,53 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>2.9114942000000001E-2</v>
-      </c>
-      <c r="B27" s="1">
-        <v>6.7303634028587697E-12</v>
-      </c>
-      <c r="C27">
-        <v>1328.4253613137801</v>
-      </c>
-      <c r="D27" s="1">
-        <v>4.8176401812824898E-11</v>
-      </c>
-      <c r="E27" s="1"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="A29">
+        <v>0.54290452899999997</v>
+      </c>
+      <c r="B29" s="1">
+        <v>5.72849099308091E-13</v>
+      </c>
+      <c r="C29">
+        <v>41.4710403851536</v>
+      </c>
+      <c r="D29">
+        <v>7.7616353713091204</v>
+      </c>
+      <c r="F29" s="1">
+        <f>AVERAGE(A29:A32)</f>
+        <v>0.55392109674999979</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" ref="G29" si="12">AVERAGE(B29:B32)</f>
+        <v>5.72849099308091E-13</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" ref="H29" si="13">AVERAGE(C29:C32)</f>
+        <v>41.4710403851536</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" ref="I29" si="14">AVERAGE(D29:D32)</f>
+        <v>7.7616353713091204</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>0.54290452899999997</v>
+        <v>0.59491184499999905</v>
       </c>
       <c r="B30" s="1">
         <v>5.72849099308091E-13</v>
@@ -6112,26 +7573,14 @@
       <c r="D30">
         <v>7.7616353713091204</v>
       </c>
-      <c r="F30" s="1">
-        <f>AVERAGE(A30:A33)</f>
-        <v>0.55392109674999979</v>
-      </c>
-      <c r="G30" s="1">
-        <f t="shared" ref="G30" si="14">AVERAGE(B30:B33)</f>
-        <v>5.72849099308091E-13</v>
-      </c>
-      <c r="H30" s="1">
-        <f t="shared" ref="H30" si="15">AVERAGE(C30:C33)</f>
-        <v>41.4710403851536</v>
-      </c>
-      <c r="I30" s="1">
-        <f t="shared" ref="I30" si="16">AVERAGE(D30:D33)</f>
-        <v>7.7616353713091204</v>
-      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>0.59491184499999905</v>
+        <v>0.53533606600000005</v>
       </c>
       <c r="B31" s="1">
         <v>5.72849099308091E-13</v>
@@ -6149,7 +7598,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>0.53533606600000005</v>
+        <v>0.54253194699999996</v>
       </c>
       <c r="B32" s="1">
         <v>5.72849099308091E-13</v>
@@ -6167,179 +7616,1121 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>0.54253194699999996</v>
+        <v>1.0670454439999999</v>
       </c>
       <c r="B33" s="1">
-        <v>5.72849099308091E-13</v>
+        <v>9.4656231829706599E-13</v>
       </c>
       <c r="C33">
-        <v>41.4710403851536</v>
+        <v>411.653612574921</v>
       </c>
       <c r="D33">
-        <v>7.7616353713091204</v>
+        <v>16.649421197107401</v>
+      </c>
+      <c r="F33" s="1">
+        <f>AVERAGE(A33:A36)</f>
+        <v>1.0403749377499998</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" ref="G33" si="15">AVERAGE(B33:B36)</f>
+        <v>9.4656231829706599E-13</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" ref="H33" si="16">AVERAGE(C33:C36)</f>
+        <v>411.653612574921</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" ref="I33" si="17">AVERAGE(D33:D36)</f>
+        <v>16.649421197107401</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>1.0129401</v>
+      </c>
+      <c r="B34" s="1">
+        <v>9.4656231829706599E-13</v>
+      </c>
+      <c r="C34">
+        <v>411.653612574921</v>
+      </c>
+      <c r="D34">
+        <v>16.649421197107401</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1.048428052</v>
+      </c>
+      <c r="B35" s="1">
+        <v>9.4656231829706599E-13</v>
+      </c>
+      <c r="C35">
+        <v>411.653612574921</v>
+      </c>
+      <c r="D35">
+        <v>16.649421197107401</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1.0330861549999999</v>
+      </c>
+      <c r="B36" s="1">
+        <v>9.4656231829706599E-13</v>
+      </c>
+      <c r="C36">
+        <v>411.653612574921</v>
+      </c>
+      <c r="D36">
+        <v>16.649421197107401</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1.8006130460000001</v>
+      </c>
+      <c r="B37" s="1">
+        <v>3.8559577310292197E-12</v>
+      </c>
+      <c r="C37">
+        <v>1328.4253613137801</v>
+      </c>
+      <c r="D37">
+        <v>34.779692853229697</v>
+      </c>
+      <c r="F37" s="1">
+        <f>AVERAGE(A37:A40)</f>
+        <v>1.9170441347500002</v>
+      </c>
+      <c r="G37" s="1">
+        <f>AVERAGE(B37:B40)</f>
+        <v>3.8559577310292197E-12</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" ref="H37" si="18">AVERAGE(C37:C40)</f>
+        <v>1328.4253613137801</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" ref="I37" si="19">AVERAGE(D37:D40)</f>
+        <v>34.779692853229697</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1.964081001</v>
+      </c>
+      <c r="B38" s="1">
+        <v>3.8559577310292197E-12</v>
+      </c>
+      <c r="C38">
+        <v>1328.4253613137801</v>
+      </c>
+      <c r="D38">
+        <v>34.779692853229697</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1.9467941390000001</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3.8559577310292197E-12</v>
+      </c>
+      <c r="C39">
+        <v>1328.4253613137801</v>
+      </c>
+      <c r="D39">
+        <v>34.779692853229697</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1.9566883530000001</v>
+      </c>
+      <c r="B40" s="1">
+        <v>3.8559577310292197E-12</v>
+      </c>
+      <c r="C40">
+        <v>1328.4253613137801</v>
+      </c>
+      <c r="D40">
+        <v>34.779692853229697</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469D2117-6EBF-4FE2-9E61-E04BD7453646}">
+  <dimension ref="A1:N50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="84" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5.7518930000000003E-2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5.03387265325499E-13</v>
+      </c>
+      <c r="C2">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7.67894014758456E-14</v>
+      </c>
+      <c r="F2" s="1">
+        <f>AVERAGE(A2:A6)</f>
+        <v>5.8098226400000008E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <f>AVERAGE(B2:B6)</f>
+        <v>5.03387265325499E-13</v>
+      </c>
+      <c r="H2" s="1">
+        <f>AVERAGE(C2:C6)</f>
+        <v>41.471548229814204</v>
+      </c>
+      <c r="I2" s="1">
+        <f>AVERAGE(D2:D6)</f>
+        <v>7.67894014758456E-14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5.7566270000000003E-2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.03387265325499E-13</v>
+      </c>
+      <c r="C3">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D3" s="1">
+        <v>7.67894014758456E-14</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5.7518432000000001E-2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.03387265325499E-13</v>
+      </c>
+      <c r="C4">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7.67894014758456E-14</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>6.2388025E-2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5.03387265325499E-13</v>
+      </c>
+      <c r="C5">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.67894014758456E-14</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5.5499475E-2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5.03387265325499E-13</v>
+      </c>
+      <c r="C6">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7.67894014758456E-14</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6.3160240000000006E-2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8.0957149060359398E-13</v>
+      </c>
+      <c r="C7">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.7108214853725802E-12</v>
+      </c>
+      <c r="F7" s="1">
+        <f>AVERAGE(A7:A11)</f>
+        <v>5.9355168600000008E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <f>AVERAGE(B7:B11)</f>
+        <v>8.0957149060359398E-13</v>
+      </c>
+      <c r="H7" s="1">
+        <f>AVERAGE(C7:C11)</f>
+        <v>411.643117448049</v>
+      </c>
+      <c r="I7" s="1">
+        <f>AVERAGE(D7:D11)</f>
+        <v>6.7108214853725802E-12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6.3237638999999998E-2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8.0957149060359398E-13</v>
+      </c>
+      <c r="C8">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6.7108214853725802E-12</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5.6976566999999999E-2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8.0957149060359398E-13</v>
+      </c>
+      <c r="C9">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6.7108214853725802E-12</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5.9171871000000001E-2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8.0957149060359398E-13</v>
+      </c>
+      <c r="C10">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6.7108214853725802E-12</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5.4229526E-2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>8.0957149060359398E-13</v>
+      </c>
+      <c r="C11">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6.7108214853725802E-12</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>7.5571783000000003E-2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3.5796018127585299E-12</v>
+      </c>
+      <c r="C12">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D12" s="1">
+        <v>6.0044160893470406E-11</v>
+      </c>
+      <c r="F12" s="1">
+        <f>AVERAGE(A12:A16)</f>
+        <v>6.7960221399999993E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <f>AVERAGE(B12:B16)</f>
+        <v>3.5796018127585299E-12</v>
+      </c>
+      <c r="H12" s="1">
+        <f>AVERAGE(C12:C16)</f>
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="I12" s="1">
+        <f>AVERAGE(D12:D16)</f>
+        <v>6.0044160893470406E-11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6.5365622999999998E-2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.5796018127585299E-12</v>
+      </c>
+      <c r="C13">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6.0044160893470406E-11</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6.5020973999999995E-2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3.5796018127585299E-12</v>
+      </c>
+      <c r="C14">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6.0044160893470406E-11</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>6.4815836000000002E-2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3.5796018127585299E-12</v>
+      </c>
+      <c r="C15">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6.0044160893470406E-11</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>6.9026891000000007E-2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3.5796018127585299E-12</v>
+      </c>
+      <c r="C16">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.0044160893470406E-11</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>7.5293231000000002E-2</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.5881159910439998E-13</v>
+      </c>
+      <c r="C19">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D19">
+        <v>7.7607424423315798</v>
+      </c>
+      <c r="F19" s="1">
+        <f>AVERAGE(A19:A23)</f>
+        <v>6.7657274200000006E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <f>AVERAGE(B19:B23)</f>
+        <v>2.5881159910439998E-13</v>
+      </c>
+      <c r="H19" s="1">
+        <f>AVERAGE(C19:C23)</f>
+        <v>41.471548229814204</v>
+      </c>
+      <c r="I19" s="1">
+        <f>AVERAGE(D19:D23)</f>
+        <v>7.7607424423315789</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>6.7765458000000001E-2</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.5881159910439998E-13</v>
+      </c>
+      <c r="C20">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D20">
+        <v>7.7607424423315798</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>6.7023418000000001E-2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.5881159910439998E-13</v>
+      </c>
+      <c r="C21">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D21">
+        <v>7.7607424423315798</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>6.2019797000000002E-2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2.5881159910439998E-13</v>
+      </c>
+      <c r="C22">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D22">
+        <v>7.7607424423315798</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6.6184466999999997E-2</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2.5881159910439998E-13</v>
+      </c>
+      <c r="C23">
+        <v>41.471548229814204</v>
+      </c>
+      <c r="D23">
+        <v>7.7607424423315798</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>7.5468273000000002E-2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4.89611016480387E-13</v>
+      </c>
+      <c r="C24">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D24">
+        <v>16.649538514358198</v>
+      </c>
+      <c r="F24" s="1">
+        <f>AVERAGE(A24:A28)</f>
+        <v>7.4333150599999995E-2</v>
+      </c>
+      <c r="G24" s="1">
+        <f>AVERAGE(B24:B28)</f>
+        <v>4.89611016480387E-13</v>
+      </c>
+      <c r="H24" s="1">
+        <f>AVERAGE(C24:C28)</f>
+        <v>411.643117448049</v>
+      </c>
+      <c r="I24" s="1">
+        <f>AVERAGE(D24:D28)</f>
+        <v>16.649538514358198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>7.8289574000000001E-2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4.89611016480387E-13</v>
+      </c>
+      <c r="C25">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D25">
+        <v>16.649538514358198</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>7.6291238999999997E-2</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4.89611016480387E-13</v>
+      </c>
+      <c r="C26">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D26">
+        <v>16.649538514358198</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>7.692148E-2</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4.89611016480387E-13</v>
+      </c>
+      <c r="C27">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D27">
+        <v>16.649538514358198</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>6.4695187000000001E-2</v>
+      </c>
+      <c r="B28" s="1">
+        <v>4.89611016480387E-13</v>
+      </c>
+      <c r="C28">
+        <v>411.643117448049</v>
+      </c>
+      <c r="D28">
+        <v>16.649538514358198</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>7.4815755999999997E-2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.87104209509251E-12</v>
+      </c>
+      <c r="C29">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D29">
+        <v>34.779802738486602</v>
+      </c>
+      <c r="F29" s="1">
+        <f>AVERAGE(A29:A33)</f>
+        <v>0.12607392079999999</v>
+      </c>
+      <c r="G29" s="1">
+        <f>AVERAGE(B29:B33)</f>
+        <v>1.87104209509251E-12</v>
+      </c>
+      <c r="H29" s="1">
+        <f>AVERAGE(C29:C33)</f>
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="I29" s="1">
+        <f>AVERAGE(D29:D33)</f>
+        <v>34.779802738486602</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0.17212776599999999</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.87104209509251E-12</v>
+      </c>
+      <c r="C30">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D30">
+        <v>34.779802738486602</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0.14376306</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.87104209509251E-12</v>
+      </c>
+      <c r="C31">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D31">
+        <v>34.779802738486602</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0.16939611700000001</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1.87104209509251E-12</v>
+      </c>
+      <c r="C32">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D32">
+        <v>34.779802738486602</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>7.0266905000000004E-2</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.87104209509251E-12</v>
+      </c>
+      <c r="C33">
+        <v>1328.3759059910999</v>
+      </c>
+      <c r="D33">
+        <v>34.779802738486602</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>1.0670454439999999</v>
-      </c>
-      <c r="B34" s="1">
-        <v>9.4656231829706599E-13</v>
-      </c>
-      <c r="C34">
-        <v>411.653612574921</v>
-      </c>
-      <c r="D34">
-        <v>16.649421197107401</v>
-      </c>
-      <c r="F34" s="1">
-        <f>AVERAGE(A34:A37)</f>
-        <v>1.0403749377499998</v>
-      </c>
-      <c r="G34" s="1">
-        <f t="shared" ref="G34" si="17">AVERAGE(B34:B37)</f>
-        <v>9.4656231829706599E-13</v>
-      </c>
-      <c r="H34" s="1">
-        <f t="shared" ref="H34" si="18">AVERAGE(C34:C37)</f>
-        <v>411.653612574921</v>
-      </c>
-      <c r="I34" s="1">
-        <f t="shared" ref="I34" si="19">AVERAGE(D34:D37)</f>
-        <v>16.649421197107401</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>1.0129401</v>
-      </c>
-      <c r="B35" s="1">
-        <v>9.4656231829706599E-13</v>
-      </c>
-      <c r="C35">
-        <v>411.653612574921</v>
-      </c>
-      <c r="D35">
-        <v>16.649421197107401</v>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>4</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>1.048428052</v>
-      </c>
-      <c r="B36" s="1">
-        <v>9.4656231829706599E-13</v>
+        <v>3.5591650029999999</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>411.653612574921</v>
+        <v>41.472232164985002</v>
       </c>
       <c r="D36">
-        <v>16.649421197107401</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <f>AVERAGE(A36:A40)</f>
+        <v>3.5542988141999983</v>
+      </c>
+      <c r="G36" s="1">
+        <f>AVERAGE(B36:B40)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <f>AVERAGE(C36:C40)</f>
+        <v>41.472232164985002</v>
+      </c>
+      <c r="I36" s="1">
+        <f>AVERAGE(D36:D40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>1.0330861549999999</v>
-      </c>
-      <c r="B37" s="1">
-        <v>9.4656231829706599E-13</v>
+        <v>3.5321843589999999</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>411.653612574921</v>
+        <v>41.472232164985002</v>
       </c>
       <c r="D37">
-        <v>16.649421197107401</v>
+        <v>0</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>1.8006130460000001</v>
-      </c>
-      <c r="B38" s="1">
-        <v>3.8559577310292197E-12</v>
+        <v>3.47616818599999</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>1328.4253613137801</v>
+        <v>41.472232164985002</v>
       </c>
       <c r="D38">
-        <v>34.779692853229697</v>
-      </c>
-      <c r="F38" s="1">
-        <f>AVERAGE(A38:A41)</f>
-        <v>1.9170441347500002</v>
-      </c>
-      <c r="G38" s="1">
-        <f>AVERAGE(B38:B41)</f>
-        <v>3.8559577310292197E-12</v>
-      </c>
-      <c r="H38" s="1">
-        <f t="shared" ref="H38" si="20">AVERAGE(C38:C41)</f>
-        <v>1328.4253613137801</v>
-      </c>
-      <c r="I38" s="1">
-        <f t="shared" ref="I38" si="21">AVERAGE(D38:D41)</f>
-        <v>34.779692853229697</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>1.964081001</v>
-      </c>
-      <c r="B39" s="1">
-        <v>3.8559577310292197E-12</v>
+        <v>3.6383126130000001</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>1328.4253613137801</v>
+        <v>41.472232164985002</v>
       </c>
       <c r="D39">
-        <v>34.779692853229697</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>1.9467941390000001</v>
-      </c>
-      <c r="B40" s="1">
-        <v>3.8559577310292197E-12</v>
+        <v>3.56566391</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
       </c>
       <c r="C40">
-        <v>1328.4253613137801</v>
+        <v>41.472232164985002</v>
       </c>
       <c r="D40">
-        <v>34.779692853229697</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>1.9566883530000001</v>
-      </c>
-      <c r="B41" s="1">
-        <v>3.8559577310292197E-12</v>
+        <v>4.939966386</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
       </c>
       <c r="C41">
-        <v>1328.4253613137801</v>
+        <v>411.63065002158902</v>
       </c>
       <c r="D41">
-        <v>34.779692853229697</v>
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <f>AVERAGE(A41:A45)</f>
+        <v>4.933981522399999</v>
+      </c>
+      <c r="G41" s="1">
+        <f>AVERAGE(B41:B45)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <f>AVERAGE(C41:C45)</f>
+        <v>411.63065002158902</v>
+      </c>
+      <c r="I41" s="1">
+        <f>AVERAGE(D41:D45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>4.8572518560000004</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>411.63065002158902</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>4.9752536809999999</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>411.63065002158902</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>4.9311524169999998</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>411.63065002158902</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="N44" s="2">
+        <f>((F46-F12)/F12)*100</f>
+        <v>7002.6097669540559</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4.9662832720000001</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>411.63065002158902</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>5.3521066929999996</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>1328.3150621909999</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <f>AVERAGE(A46:A50)</f>
+        <v>4.8269493228</v>
+      </c>
+      <c r="G46" s="1">
+        <f>AVERAGE(B46:B50)</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
+        <f>AVERAGE(C46:C50)</f>
+        <v>1328.3150621909999</v>
+      </c>
+      <c r="I46" s="1">
+        <f>AVERAGE(D46:D50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>4.4766684730000001</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>1328.3150621909999</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>4.4217643559999997</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>1328.3150621909999</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>4.4280517440000002</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>1328.3150621909999</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>5.4561553480000002</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>1328.3150621909999</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A36:D50">
+    <sortCondition ref="C36:C50"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>